<commit_message>
data base migration from mysql to postgres. defect fix: If consumption for current mont does not exist create consumption autmation related changes
</commit_message>
<xml_diff>
--- a/data/test/TestSet1.xlsx
+++ b/data/test/TestSet1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>Test ID</t>
   </si>
@@ -330,6 +330,78 @@
   </si>
   <si>
     <t>//*[@id='list-category']/li</t>
+  </si>
+  <si>
+    <t>FIND</t>
+  </si>
+  <si>
+    <t>//*[@id='btn-edit-category']</t>
+  </si>
+  <si>
+    <t>CLICK</t>
+  </si>
+  <si>
+    <t>SINGLE</t>
+  </si>
+  <si>
+    <t>MULTIPLE</t>
+  </si>
+  <si>
+    <t>OCCURENCE</t>
+  </si>
+  <si>
+    <t>ELEMENT NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tes </t>
+  </si>
+  <si>
+    <t>TEST Category 10</t>
+  </si>
+  <si>
+    <t>//*[@id='form-edit-category']/div[]</t>
+  </si>
+  <si>
+    <t>//*[@id='form-edit-category']/div[2]/div/span/input[@name='name']</t>
+  </si>
+  <si>
+    <t>click nth edit button</t>
+  </si>
+  <si>
+    <t>enter new category value</t>
+  </si>
+  <si>
+    <t>//*[@id='btn-edit-submit']</t>
+  </si>
+  <si>
+    <t>Submit form</t>
+  </si>
+  <si>
+    <t>Search for edited valued</t>
+  </si>
+  <si>
+    <t>Search for updated value</t>
+  </si>
+  <si>
+    <t>Test Category 3</t>
+  </si>
+  <si>
+    <t>Test Category 4</t>
+  </si>
+  <si>
+    <t>//*[@id='form-edit-category']</t>
+  </si>
+  <si>
+    <t>//*[@id='btn-edit-category-0']</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>MULTIPLE</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1272,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.000000"/>
@@ -1306,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -1317,12 +1389,14 @@
     <col min="1" max="1" width="6.88000011" customWidth="1" outlineLevel="0"/>
     <col min="2" max="2" width="22.75499916" customWidth="1" outlineLevel="0"/>
     <col min="4" max="5" width="9.00500011" customWidth="1" outlineLevel="0"/>
-    <col min="6" max="6" width="54.63000107" customWidth="1" outlineLevel="0"/>
-    <col min="7" max="7" width="27.37999916" customWidth="1" outlineLevel="0"/>
-    <col min="9" max="9" width="19.37999916" customWidth="1" outlineLevel="0"/>
+    <col min="6" max="6" width="9.00500011" customWidth="1" outlineLevel="0"/>
+    <col min="7" max="7" width="12.63000011" customWidth="1" outlineLevel="0"/>
+    <col min="8" max="8" width="54.63000107" customWidth="1" outlineLevel="0"/>
+    <col min="9" max="9" width="27.37999916" customWidth="1" outlineLevel="0"/>
+    <col min="11" max="11" width="19.37999916" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="0" t="s">
         <v>29</v>
       </c>
@@ -1339,13 +1413,19 @@
         <v>89</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2" s="0">
         <v>1</v>
       </c>
@@ -1361,14 +1441,17 @@
       <c r="E2" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="0">
         <v>1</v>
       </c>
@@ -1382,14 +1465,17 @@
         <v>55</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="0">
         <v>1</v>
       </c>
@@ -1403,13 +1489,16 @@
         <v>55</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="A5" s="0">
         <v>1</v>
       </c>
@@ -1422,11 +1511,14 @@
       <c r="D5" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:11">
       <c r="A6" s="0">
         <v>1</v>
       </c>
@@ -1442,14 +1534,17 @@
       <c r="E6" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="I6" s="0" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:11">
       <c r="A7" s="0">
         <v>1</v>
       </c>
@@ -1462,14 +1557,17 @@
       <c r="D7" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="I7" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:11">
       <c r="A8" s="0">
         <v>2</v>
       </c>
@@ -1485,14 +1583,17 @@
       <c r="E8" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="I8" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:11">
       <c r="A9" s="0">
         <v>2</v>
       </c>
@@ -1505,11 +1606,14 @@
       <c r="D9" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:11">
       <c r="A10" s="0">
         <v>2</v>
       </c>
@@ -1522,14 +1626,17 @@
       <c r="D10" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="I10" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="0">
         <v>2</v>
       </c>
@@ -1543,10 +1650,13 @@
         <v>96</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" s="0" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:11">
       <c r="A12" s="0">
         <v>2</v>
       </c>
@@ -1562,11 +1672,14 @@
       <c r="E12" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:11">
       <c r="A13" s="0">
         <v>2</v>
       </c>
@@ -1579,27 +1692,174 @@
       <c r="D13" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>102</v>
+      <c r="I13" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16.500000" customHeight="1">
+      <c r="A14" s="0">
+        <v>3</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="0">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="0">
+        <v>3</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="0">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" s="0">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="0">
+        <v>3</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="0">
+        <v>2</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="0">
+        <v>3</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="0">
+        <v>3</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16.500000" customHeight="1">
+      <c r="A18" s="0">
+        <v>2</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="0">
+        <v>5</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="0">
+        <v>3</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="0">
+        <v>4</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId0" ref="G3"/>
-    <hyperlink r:id="rId1" ref="G4"/>
-    <hyperlink r:id="rId2" ref="F2"/>
-    <hyperlink r:id="rId3" ref="F6"/>
-    <hyperlink r:id="rId4" ref="F7"/>
-    <hyperlink r:id="rId5" ref="F8"/>
-    <hyperlink r:id="rId6" ref="F9"/>
-    <hyperlink r:id="rId7" ref="F10"/>
-    <hyperlink r:id="rId8" ref="F12"/>
-    <hyperlink r:id="rId9" ref="F5"/>
-    <hyperlink r:id="rId10" ref="F13"/>
+    <hyperlink r:id="rId0" ref="I3"/>
+    <hyperlink r:id="rId1" ref="I4"/>
+    <hyperlink r:id="rId2" ref="H2"/>
+    <hyperlink r:id="rId3" ref="H6"/>
+    <hyperlink r:id="rId4" ref="H7"/>
+    <hyperlink r:id="rId5" ref="H8"/>
+    <hyperlink r:id="rId6" ref="H9"/>
+    <hyperlink r:id="rId7" ref="H10"/>
+    <hyperlink r:id="rId8" ref="H12"/>
+    <hyperlink r:id="rId9" ref="H5"/>
+    <hyperlink r:id="rId10" ref="H13"/>
+    <hyperlink r:id="rId11" ref="H16"/>
+    <hyperlink r:id="rId12" ref="H17"/>
+    <hyperlink r:id="rId13" ref="H19"/>
+    <hyperlink r:id="rId14" ref="H18"/>
+    <hyperlink r:id="rId15" ref="H14"/>
+    <hyperlink r:id="rId16" ref="H15"/>
   </hyperlinks>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1619,7 +1879,7 @@
     <col min="2" max="2" width="50.13000107" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="16.500000">
       <c r="A1" s="0" t="s">
         <v>9</v>
       </c>
@@ -1627,7 +1887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="16.500000">
       <c r="A2" s="0">
         <v>1001</v>
       </c>

</xml_diff>